<commit_message>
data provider methode change
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/OrangeHrm.xlsx
+++ b/src/test/resources/ExcelSheet/OrangeHrm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\automation\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2307B113-BBD6-4EB0-824B-E7F6823C5AEB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC2D173-12DA-4247-B951-6145029B69E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="10890" activeTab="2" xr2:uid="{3DDDAB6D-2287-4D35-8AC7-D3D60F9E8391}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Attendance record with date picker 3 test done
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/OrangeHrm.xlsx
+++ b/src/test/resources/ExcelSheet/OrangeHrm.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\automation\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC2D173-12DA-4247-B951-6145029B69E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644E5D5-F04C-4F70-8313-BEE91F356034}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="10890" activeTab="2" xr2:uid="{3DDDAB6D-2287-4D35-8AC7-D3D60F9E8391}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="10890" activeTab="3" xr2:uid="{3DDDAB6D-2287-4D35-8AC7-D3D60F9E8391}"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="2" r:id="rId1"/>
     <sheet name="Trackers" sheetId="3" r:id="rId2"/>
     <sheet name="PerfomanceReview" sheetId="4" r:id="rId3"/>
+    <sheet name="AttendanceRecord" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>jobTitle</t>
   </si>
@@ -78,6 +79,9 @@
   </si>
   <si>
     <t>Linda</t>
+  </si>
+  <si>
+    <t>Linda Anderson</t>
   </si>
 </sst>
 </file>
@@ -544,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1883161-A496-4D6B-976B-8B595A3BD309}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,4 +599,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53C443F-4452-4D53-B2D4-563E7AA15B1B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
search KPIs test and edit trackers
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/OrangeHrm.xlsx
+++ b/src/test/resources/ExcelSheet/OrangeHrm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\automation\data-driven-test-automation\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0644E5D5-F04C-4F70-8313-BEE91F356034}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC4B098-1FFD-4763-BD8B-FEF6F3A8F8CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="10890" activeTab="3" xr2:uid="{3DDDAB6D-2287-4D35-8AC7-D3D60F9E8391}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="KPI" sheetId="2" r:id="rId1"/>
     <sheet name="Trackers" sheetId="3" r:id="rId2"/>
     <sheet name="PerfomanceReview" sheetId="4" r:id="rId3"/>
-    <sheet name="AttendanceRecord" sheetId="5" r:id="rId4"/>
+    <sheet name="EditTrackers" sheetId="6" r:id="rId4"/>
+    <sheet name="AttendanceRecord" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>jobTitle</t>
   </si>
@@ -78,10 +79,13 @@
     <t>dueDate</t>
   </si>
   <si>
-    <t>Linda</t>
-  </si>
-  <si>
     <t>Linda Anderson</t>
+  </si>
+  <si>
+    <t>Thomas Fleming</t>
+  </si>
+  <si>
+    <t>charushila mahajan</t>
   </si>
 </sst>
 </file>
@@ -91,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +114,12 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -140,6 +150,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +517,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +560,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,10 +613,53 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1A8480-75AB-450B-9601-670CD9AAA213}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53C443F-4452-4D53-B2D4-563E7AA15B1B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -621,7 +675,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>